<commit_message>
Added more columns for more specific information collection
</commit_message>
<xml_diff>
--- a/Hospital ER.xlsx
+++ b/Hospital ER.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="27">
   <si>
     <t>Patient ID</t>
   </si>
@@ -24,9 +24,6 @@
     <t>Priority</t>
   </si>
   <si>
-    <t>Completion Time(hrs)</t>
-  </si>
-  <si>
     <t>High</t>
   </si>
   <si>
@@ -34,6 +31,72 @@
   </si>
   <si>
     <t>Low</t>
+  </si>
+  <si>
+    <t>Operation Completion Time(hrs)</t>
+  </si>
+  <si>
+    <t>Patient Name</t>
+  </si>
+  <si>
+    <t>Admission date</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>Admission type</t>
+  </si>
+  <si>
+    <t>Kendric Lamar</t>
+  </si>
+  <si>
+    <t>Sean Chini</t>
+  </si>
+  <si>
+    <t>Jonathan Cole</t>
+  </si>
+  <si>
+    <t>Patrick Star</t>
+  </si>
+  <si>
+    <t>Mike Killer</t>
+  </si>
+  <si>
+    <t>Taona Munikwa</t>
+  </si>
+  <si>
+    <t>Tariro Gezi</t>
+  </si>
+  <si>
+    <t>Mukudzei Mukombe</t>
+  </si>
+  <si>
+    <t>Joe Budden</t>
+  </si>
+  <si>
+    <t>Kevin Hart</t>
+  </si>
+  <si>
+    <t>Beyonce</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Doja cat</t>
+  </si>
+  <si>
+    <t>Planned</t>
+  </si>
+  <si>
+    <t>Unplanned</t>
   </si>
 </sst>
 </file>
@@ -69,8 +132,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -372,160 +436,359 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" customWidth="1"/>
-    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="3" max="4" width="8.42578125" customWidth="1"/>
+    <col min="5" max="5" width="30.85546875" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2">
+        <v>41</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1">
+        <v>45372</v>
+      </c>
+      <c r="H2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="1">
+        <v>45371</v>
+      </c>
+      <c r="H3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1">
+        <v>45370</v>
+      </c>
+      <c r="H4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="1">
+        <v>45372</v>
+      </c>
+      <c r="H5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6">
         <v>3</v>
       </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="1">
+        <v>45372</v>
+      </c>
+      <c r="H6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7">
+        <v>61</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7">
         <v>1</v>
       </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="1">
+        <v>45369</v>
+      </c>
+      <c r="H7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8">
         <v>5</v>
       </c>
-      <c r="C8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="1">
+        <v>45372</v>
+      </c>
+      <c r="H8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9">
+        <v>28</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9">
         <v>3</v>
       </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="1">
+        <v>45371</v>
+      </c>
+      <c r="H9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10">
         <v>6</v>
       </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="1">
+        <v>45371</v>
+      </c>
+      <c r="H10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11">
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11">
+        <v>48</v>
+      </c>
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11">
         <v>1</v>
       </c>
-      <c r="C11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" s="1">
+        <v>45372</v>
+      </c>
+      <c r="H11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12">
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12">
+        <v>37</v>
+      </c>
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12">
         <v>2</v>
       </c>
-      <c r="C12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" s="1">
+        <v>45371</v>
+      </c>
+      <c r="H12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13">
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13">
+        <v>20</v>
+      </c>
+      <c r="D13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13">
         <v>1</v>
       </c>
-      <c r="C13" t="s">
-        <v>4</v>
+      <c r="F13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" s="1">
+        <v>45370</v>
+      </c>
+      <c r="H13" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>